<commit_message>
Draft: 5th tentative fully functional advanced control taxa removal
On branch advCtrl
Changes to be committed:
	modified:   recentrifuge/core.py
	modified:   recentrifuge/rank.py
	modified:   remock.py
	modified:   test/mock.xlsx
</commit_message>
<xml_diff>
--- a/test/mock.xlsx
+++ b/test/mock.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="2440" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="3180" yWindow="22060" windowWidth="20780" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="mock" sheetId="1" r:id="rId1"/>
+    <sheet name="notes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -65,9 +66,6 @@
     <t>Lactobacillus helveticus</t>
   </si>
   <si>
-    <t xml:space="preserve"> T5virus</t>
-  </si>
-  <si>
     <t>Salmonella virus Stitch</t>
   </si>
   <si>
@@ -114,13 +112,37 @@
   </si>
   <si>
     <t>Comamonadaceae</t>
+  </si>
+  <si>
+    <t>SUM (this row is ignored)</t>
+  </si>
+  <si>
+    <t>collapsed &lt; 5</t>
+  </si>
+  <si>
+    <t>severe &gt; 100 any</t>
+  </si>
+  <si>
+    <t>mild &gt; 10 all</t>
+  </si>
+  <si>
+    <t>5 &lt;= others &lt;= 10 all &lt; 100 any</t>
+  </si>
+  <si>
+    <t>CONTAMINATION RULES:</t>
+  </si>
+  <si>
+    <t>smpl4</t>
+  </si>
+  <si>
+    <t>T5virus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -135,13 +157,61 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -156,9 +226,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" zoomScalePageLayoutView="126" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -447,320 +525,356 @@
     <col min="1" max="1" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>24</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>9606</v>
       </c>
       <c r="C2">
-        <v>600</v>
+        <v>9650</v>
       </c>
       <c r="D2">
-        <v>500</v>
+        <v>7000</v>
       </c>
       <c r="E2">
-        <v>400</v>
+        <v>9650</v>
       </c>
       <c r="F2">
-        <v>300</v>
+        <v>4400</v>
       </c>
       <c r="G2">
-        <v>250</v>
+        <v>3800</v>
       </c>
       <c r="H2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+        <v>2900</v>
+      </c>
+      <c r="I2">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>1747</v>
       </c>
       <c r="C3">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="D3">
-        <v>250</v>
+        <v>2800</v>
       </c>
       <c r="E3">
-        <v>250</v>
+        <v>5</v>
       </c>
       <c r="F3">
+        <v>1000</v>
+      </c>
+      <c r="G3">
+        <v>1000</v>
+      </c>
+      <c r="H3">
+        <v>1000</v>
+      </c>
+      <c r="I3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>9598</v>
+      </c>
+      <c r="C4">
         <v>100</v>
       </c>
-      <c r="G3">
-        <v>100</v>
-      </c>
-      <c r="H3">
+      <c r="D4">
+        <v>11</v>
+      </c>
+      <c r="E4">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="F4">
+        <v>500</v>
+      </c>
+      <c r="G4">
+        <v>500</v>
+      </c>
+      <c r="H4">
+        <v>500</v>
+      </c>
+      <c r="I4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>562</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>50</v>
-      </c>
-      <c r="D4">
-        <v>50</v>
-      </c>
-      <c r="E4">
-        <v>6</v>
-      </c>
-      <c r="F4">
-        <v>50</v>
-      </c>
-      <c r="G4">
-        <v>50</v>
-      </c>
-      <c r="H4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>4577</v>
-      </c>
-      <c r="C5">
-        <v>25</v>
       </c>
       <c r="D5">
         <v>50</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="F5">
-        <v>20</v>
+        <v>500</v>
       </c>
       <c r="G5">
-        <v>20</v>
+        <v>500</v>
       </c>
       <c r="H5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>500</v>
+      </c>
+      <c r="I5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>4565</v>
+        <v>4577</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="D6">
         <v>50</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>4565</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>49</v>
+      </c>
+      <c r="E7">
+        <v>40</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>425265</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
         <v>20</v>
       </c>
-      <c r="G6">
-        <v>20</v>
-      </c>
-      <c r="H6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>425265</v>
-      </c>
-      <c r="C7">
-        <v>25</v>
-      </c>
-      <c r="D7">
-        <v>25</v>
-      </c>
-      <c r="E7">
+      <c r="E8">
         <v>100</v>
       </c>
-      <c r="F7">
-        <v>50</v>
-      </c>
-      <c r="G7">
-        <v>50</v>
-      </c>
-      <c r="H7">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>9598</v>
-      </c>
-      <c r="C8">
-        <v>25</v>
-      </c>
-      <c r="D8">
-        <v>25</v>
-      </c>
-      <c r="E8">
-        <v>200</v>
-      </c>
       <c r="F8">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="G8">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="H8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="I8">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B9">
         <v>1655020</v>
       </c>
       <c r="C9">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="D9">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G9">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="H9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B10">
         <v>2209</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D10">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E10">
         <v>10</v>
       </c>
       <c r="F10">
-        <v>300</v>
+        <v>2000</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>2208</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <v>500</v>
+      </c>
+      <c r="I11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>1578</v>
       </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
         <v>10</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>15</v>
-      </c>
-      <c r="F11">
-        <v>50</v>
-      </c>
-      <c r="G11">
-        <v>50</v>
-      </c>
-      <c r="H11">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>2208</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
       </c>
       <c r="F12">
         <v>50</v>
       </c>
       <c r="G12">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="H12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="I12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B13">
@@ -773,21 +887,24 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="G13">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="H13">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>400</v>
+      </c>
+      <c r="I13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="B14">
         <v>187218</v>
@@ -802,18 +919,21 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>426</v>
       </c>
       <c r="G14">
-        <v>50</v>
+        <v>524</v>
       </c>
       <c r="H14">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>471</v>
+      </c>
+      <c r="I14">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="B15">
         <v>1540099</v>
@@ -831,15 +951,18 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
+      <c r="I15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="B16">
         <v>28901</v>
@@ -857,15 +980,18 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>15</v>
+      <c r="I16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="B17">
         <v>54736</v>
@@ -883,15 +1009,18 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>46</v>
+        <v>500</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
+      <c r="I17">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="B18">
         <v>59201</v>
@@ -909,15 +1038,18 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>25</v>
+      <c r="I18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="B19">
         <v>31998</v>
@@ -932,18 +1064,21 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>5</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="B20">
         <v>398578</v>
@@ -964,12 +1099,15 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>500</v>
+      </c>
+      <c r="I20">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="B21">
         <v>80865</v>
@@ -990,12 +1128,15 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>1000</v>
+      </c>
+      <c r="I21">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="B22">
         <v>80864</v>
@@ -1016,7 +1157,86 @@
         <v>0</v>
       </c>
       <c r="H22">
-        <v>100</v>
+        <v>1000</v>
+      </c>
+      <c r="I22">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23">
+        <f>SUM(C2:C22)</f>
+        <v>10000</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ref="D23:I23" si="0">SUM(D2:D22)</f>
+        <v>10000</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fully functional, improved summary of samples in parallel (to 0.16.0)
On branch summary
Changes to be committed:
	modified:   recentrifuge.py
	modified:   recentrifuge/centrifuge.py
	modified:   recentrifuge/config.py
	modified:   recentrifuge/core.py
	modified:   recentrifuge/krona.js
	modified:   recentrifuge/rank.py
	modified:   test/mock.xlsx
</commit_message>
<xml_diff>
--- a/test/mock.xlsx
+++ b/test/mock.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="22060" windowWidth="20780" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="3200" yWindow="22080" windowWidth="20780" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="mock" sheetId="1" r:id="rId1"/>
@@ -164,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,6 +213,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -226,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -237,6 +243,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,7 +524,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" zoomScalePageLayoutView="126" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -986,11 +993,11 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>500</v>
+        <v>750</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B17">
@@ -1015,7 +1022,7 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>250</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Solve score calculation bug in allin1 (to _rc9)
On branch summary
Changes to be committed:
	modified:   recentrifuge.py
	modified:   recentrifuge/centrifuge.py
	modified:   recentrifuge/krona.js
	modified:   recentrifuge/trees.py
	modified:   test/mock.xlsx
</commit_message>
<xml_diff>
--- a/test/mock.xlsx
+++ b/test/mock.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="22080" windowWidth="20780" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="4120" yWindow="22560" windowWidth="20780" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="mock" sheetId="1" r:id="rId1"/>
@@ -164,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,6 +219,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -232,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -244,6 +250,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,7 +531,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" zoomScalePageLayoutView="126" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -717,7 +724,7 @@
         <v>30</v>
       </c>
       <c r="D7">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E7">
         <v>40</v>
@@ -833,7 +840,7 @@
         <v>6</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E11">
         <v>8</v>
@@ -881,7 +888,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B13">
@@ -910,7 +917,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B14">
@@ -1055,7 +1062,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B19">

</xml_diff>

<commit_message>
Add flag to remove ROOT counts and scores (to 0.17.2)
On branch advCtrl
Your branch is up-to-date with 'origin/advCtrl'.

Changes to be committed:
	modified:   recentrifuge.py
	modified:   recentrifuge/centrifuge.py
	modified:   test/mock.xlsx
</commit_message>
<xml_diff>
--- a/test/mock.xlsx
+++ b/test/mock.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>T5virus</t>
+  </si>
+  <si>
+    <t>Root</t>
   </si>
 </sst>
 </file>
@@ -238,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -251,6 +254,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" zoomScalePageLayoutView="126" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -576,25 +580,25 @@
         <v>9606</v>
       </c>
       <c r="C2">
-        <v>9650</v>
+        <v>8650</v>
       </c>
       <c r="D2">
-        <v>7000</v>
+        <v>6000</v>
       </c>
       <c r="E2">
-        <v>9650</v>
+        <v>8650</v>
       </c>
       <c r="F2">
-        <v>4400</v>
+        <v>3400</v>
       </c>
       <c r="G2">
-        <v>3800</v>
+        <v>2800</v>
       </c>
       <c r="H2">
-        <v>2900</v>
+        <v>1900</v>
       </c>
       <c r="I2">
-        <v>3000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1178,35 +1182,64 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1000</v>
+      </c>
+      <c r="D23">
+        <v>1000</v>
+      </c>
+      <c r="E23">
+        <v>1000</v>
+      </c>
+      <c r="F23">
+        <v>1000</v>
+      </c>
+      <c r="G23">
+        <v>1000</v>
+      </c>
+      <c r="H23">
+        <v>1000</v>
+      </c>
+      <c r="I23">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C23">
-        <f>SUM(C2:C22)</f>
+      <c r="C24">
+        <f>SUM(C2:C23)</f>
         <v>10000</v>
       </c>
-      <c r="D23">
-        <f t="shared" ref="D23:I23" si="0">SUM(D2:D22)</f>
+      <c r="D24">
+        <f>SUM(D2:D23)</f>
         <v>10000</v>
       </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
+      <c r="E24">
+        <f>SUM(E2:E23)</f>
         <v>10000</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="0"/>
+      <c r="F24">
+        <f>SUM(F2:F23)</f>
         <v>10000</v>
       </c>
-      <c r="G23">
-        <f t="shared" si="0"/>
+      <c r="G24">
+        <f>SUM(G2:G23)</f>
         <v>10000</v>
       </c>
-      <c r="H23">
-        <f t="shared" si="0"/>
+      <c r="H24">
+        <f>SUM(H2:H23)</f>
         <v>10000</v>
       </c>
-      <c r="I23">
-        <f t="shared" si="0"/>
+      <c r="I24">
+        <f>SUM(I2:I23)</f>
         <v>10000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve crossover detection in advCtrl (to 0.17.3_rc3)
On branch advCtrl
Changes to be committed:
	modified:   recentrifuge/config.py
	modified:   recentrifuge/core.py
	modified:   test/mock.xlsx
</commit_message>
<xml_diff>
--- a/test/mock.xlsx
+++ b/test/mock.xlsx
@@ -535,7 +535,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" zoomScalePageLayoutView="126" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -595,7 +595,7 @@
         <v>2800</v>
       </c>
       <c r="H2">
-        <v>1900</v>
+        <v>1800</v>
       </c>
       <c r="I2">
         <v>2000</v>
@@ -847,7 +847,7 @@
         <v>4</v>
       </c>
       <c r="E11">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -856,7 +856,7 @@
         <v>7</v>
       </c>
       <c r="H11">
-        <v>500</v>
+        <v>601</v>
       </c>
       <c r="I11">
         <v>15</v>
@@ -905,7 +905,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F13">
         <v>600</v>
@@ -943,7 +943,7 @@
         <v>524</v>
       </c>
       <c r="H14">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I14">
         <v>486</v>

</xml_diff>

<commit_message>
Correct and update rextract and add minscore option (to 0.2.0)
On branch advCtrl
Changes to be committed:
	modified:   recentrifuge/centrifuge.py
	modified:   recentrifuge/config.py
	modified:   recentrifuge/trees.py
	modified:   rextract.py
	modified:   test/mock.xlsx
</commit_message>
<xml_diff>
--- a/test/mock.xlsx
+++ b/test/mock.xlsx
@@ -1215,31 +1215,31 @@
         <v>28</v>
       </c>
       <c r="C24">
-        <f>SUM(C2:C23)</f>
+        <f t="shared" ref="C24:I24" si="0">SUM(C2:C23)</f>
         <v>10000</v>
       </c>
       <c r="D24">
-        <f>SUM(D2:D23)</f>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="E24">
-        <f>SUM(E2:E23)</f>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="F24">
-        <f>SUM(F2:F23)</f>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="G24">
-        <f>SUM(G2:G23)</f>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="H24">
-        <f>SUM(H2:H23)</f>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="I24">
-        <f>SUM(I2:I23)</f>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update test dataset data and add results for validation
On branch master
	modified:   recentrifuge.py
	new file:   test/TEST.rcf.html
	new file:   test/TEST.rcf.txt
	new file:   test/TEST.rcf.xlsx
	modified:   test/mock.xlsx
</commit_message>
<xml_diff>
--- a/test/mock.xlsx
+++ b/test/mock.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="22560" windowWidth="20780" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="5620" yWindow="2480" windowWidth="22680" windowHeight="16580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="mock" sheetId="1" r:id="rId1"/>
@@ -145,7 +145,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -164,6 +164,12 @@
       <i/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -534,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" zoomScalePageLayoutView="126" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="126" zoomScaleNormal="126" zoomScalePageLayoutView="126" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,25 +586,25 @@
         <v>9606</v>
       </c>
       <c r="C2">
-        <v>8650</v>
+        <v>86644</v>
       </c>
       <c r="D2">
-        <v>6000</v>
+        <v>60126</v>
       </c>
       <c r="E2">
-        <v>8650</v>
+        <v>86644</v>
       </c>
       <c r="F2">
-        <v>3400</v>
+        <v>34090</v>
       </c>
       <c r="G2">
-        <v>2800</v>
+        <v>28243</v>
       </c>
       <c r="H2">
-        <v>1800</v>
+        <v>18189</v>
       </c>
       <c r="I2">
-        <v>2000</v>
+        <v>20315</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -609,25 +615,25 @@
         <v>1747</v>
       </c>
       <c r="C3">
+        <v>500</v>
+      </c>
+      <c r="D3">
+        <v>28000</v>
+      </c>
+      <c r="E3">
         <v>50</v>
       </c>
-      <c r="D3">
-        <v>2800</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
       <c r="F3">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="G3">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="H3">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="I3">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -638,25 +644,25 @@
         <v>9598</v>
       </c>
       <c r="C4">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="D4">
-        <v>11</v>
+        <v>110</v>
       </c>
       <c r="E4">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="F4">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="G4">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="H4">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="I4">
-        <v>500</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -667,25 +673,25 @@
         <v>562</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="D5">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="E5">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="F5">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="G5">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="H5">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="I5">
-        <v>500</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -696,25 +702,25 @@
         <v>4577</v>
       </c>
       <c r="C6">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="D6">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="E6">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="I6">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -725,13 +731,13 @@
         <v>4565</v>
       </c>
       <c r="C7">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="D7">
-        <v>45</v>
+        <v>450</v>
       </c>
       <c r="E7">
-        <v>40</v>
+        <v>400</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -757,22 +763,22 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="E8">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F8">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="G8">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="H8">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="I8">
-        <v>500</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -783,25 +789,25 @@
         <v>1655020</v>
       </c>
       <c r="C9">
+        <v>500</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>200</v>
+      </c>
+      <c r="F9">
         <v>50</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>20</v>
-      </c>
-      <c r="F9">
-        <v>5</v>
-      </c>
       <c r="G9">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H9">
-        <v>200</v>
+        <v>2000</v>
       </c>
       <c r="I9">
-        <v>200</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -821,7 +827,7 @@
         <v>10</v>
       </c>
       <c r="F10">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="G10">
         <v>20</v>
@@ -856,7 +862,7 @@
         <v>7</v>
       </c>
       <c r="H11">
-        <v>601</v>
+        <v>6001</v>
       </c>
       <c r="I11">
         <v>15</v>
@@ -870,25 +876,25 @@
         <v>1578</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E12">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="F12">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="G12">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="H12">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="I12">
-        <v>500</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -905,19 +911,19 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F13">
-        <v>600</v>
+        <v>6000</v>
       </c>
       <c r="G13">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="H13">
-        <v>400</v>
+        <v>4000</v>
       </c>
       <c r="I13">
-        <v>500</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -937,16 +943,16 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>426</v>
+        <v>4260</v>
       </c>
       <c r="G14">
-        <v>524</v>
+        <v>5240</v>
       </c>
       <c r="H14">
-        <v>470</v>
+        <v>4700</v>
       </c>
       <c r="I14">
-        <v>486</v>
+        <v>4860</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -969,13 +975,13 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>500</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -998,13 +1004,13 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>750</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1027,7 +1033,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1056,13 +1062,13 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>40</v>
+        <v>400</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>20</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1082,16 +1088,16 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="G19">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="H19">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="I19">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1117,10 +1123,10 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="I20">
-        <v>500</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1146,10 +1152,10 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="I21">
-        <v>500</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1175,10 +1181,10 @@
         <v>0</v>
       </c>
       <c r="H22">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="I22">
-        <v>500</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1189,25 +1195,25 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="D23">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="E23">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="F23">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="G23">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="H23">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="I23">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1216,35 +1222,37 @@
       </c>
       <c r="C24">
         <f t="shared" ref="C24:I24" si="0">SUM(C2:C23)</f>
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="H24">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="I24">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>100000</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1287,6 +1295,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Further update test dataset and validation results
On branch master
	modified:   test/TEST.rcf.html
	modified:   test/TEST.rcf.txt
	modified:   test/TEST.rcf.xlsx
	modified:   test/mock.xlsx
</commit_message>
<xml_diff>
--- a/test/mock.xlsx
+++ b/test/mock.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="2480" windowWidth="22680" windowHeight="16580" tabRatio="500"/>
+    <workbookView xWindow="6120" yWindow="22060" windowWidth="26340" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="mock" sheetId="1" r:id="rId1"/>
@@ -117,9 +117,6 @@
     <t>SUM (this row is ignored)</t>
   </si>
   <si>
-    <t>collapsed &lt; 5</t>
-  </si>
-  <si>
     <t>severe &gt; 100 any</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>Root</t>
+  </si>
+  <si>
+    <t>collapsed &lt; mintaxa (5)</t>
   </si>
 </sst>
 </file>
@@ -540,9 +540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="126" zoomScaleNormal="126" zoomScalePageLayoutView="126" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:I30"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" zoomScalePageLayoutView="126" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -575,7 +573,7 @@
         <v>21</v>
       </c>
       <c r="I1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -586,25 +584,25 @@
         <v>9606</v>
       </c>
       <c r="C2">
-        <v>86644</v>
+        <v>87130</v>
       </c>
       <c r="D2">
-        <v>60126</v>
+        <v>60576</v>
       </c>
       <c r="E2">
-        <v>86644</v>
+        <v>87130</v>
       </c>
       <c r="F2">
-        <v>34090</v>
+        <v>34171</v>
       </c>
       <c r="G2">
-        <v>28243</v>
+        <v>28324</v>
       </c>
       <c r="H2">
-        <v>18189</v>
+        <v>18270</v>
       </c>
       <c r="I2">
-        <v>20315</v>
+        <v>20396</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -702,25 +700,25 @@
         <v>4577</v>
       </c>
       <c r="C6">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="D6">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="E6">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="F6">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="G6">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="H6">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="I6">
-        <v>40</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -876,7 +874,7 @@
         <v>1578</v>
       </c>
       <c r="C12">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="D12">
         <v>100</v>
@@ -911,7 +909,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="F13">
         <v>6000</v>
@@ -928,7 +926,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>187218</v>
@@ -1088,16 +1086,16 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="G19">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="H19">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="I19">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1189,7 +1187,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1261,7 +1259,7 @@
   <dimension ref="A4:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1271,27 +1269,27 @@
   <sheetData>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add types of contamination key sheet to test/mock.xlsx
On branch master
	modified:   test/mock.xlsx
</commit_message>
<xml_diff>
--- a/test/mock.xlsx
+++ b/test/mock.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="22060" windowWidth="26340" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="6120" yWindow="22060" windowWidth="26340" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="mock" sheetId="1" r:id="rId1"/>
-    <sheet name="notes" sheetId="2" r:id="rId2"/>
+    <sheet name="types" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -117,18 +117,6 @@
     <t>SUM (this row is ignored)</t>
   </si>
   <si>
-    <t>severe &gt; 100 any</t>
-  </si>
-  <si>
-    <t>mild &gt; 10 all</t>
-  </si>
-  <si>
-    <t>5 &lt;= others &lt;= 10 all &lt; 100 any</t>
-  </si>
-  <si>
-    <t>CONTAMINATION RULES:</t>
-  </si>
-  <si>
     <t>smpl4</t>
   </si>
   <si>
@@ -138,14 +126,68 @@
     <t>Root</t>
   </si>
   <si>
-    <t>collapsed &lt; mintaxa (5)</t>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>Severe</t>
+  </si>
+  <si>
+    <t>Mild</t>
+  </si>
+  <si>
+    <t>Just CTRL</t>
+  </si>
+  <si>
+    <t>Crossover</t>
+  </si>
+  <si>
+    <t>NO contamination</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>SEVR_CONTM_MIN_RELFREQ</t>
+  </si>
+  <si>
+    <t>if all relfreq &gt; SEVR_CONTM_MIN_RELFREQ</t>
+  </si>
+  <si>
+    <t>if any relfreq &gt; SEVR_CONTM_MIN_RELFREQ</t>
+  </si>
+  <si>
+    <t>if all relfreq &gt; MILD_CONTM_MIN_RELFREQ</t>
+  </si>
+  <si>
+    <t>not present in samples, just in any control</t>
+  </si>
+  <si>
+    <t>not in a case above</t>
+  </si>
+  <si>
+    <t>not in any control sample (beyond mintaxa)</t>
+  </si>
+  <si>
+    <t>TYPES OF CONTAMINANTS AND RULES</t>
+  </si>
+  <si>
+    <t>passes both checks of the crossover test</t>
+  </si>
+  <si>
+    <t>DEFAULT VALUES</t>
+  </si>
+  <si>
+    <t>MILD_CONTM_MIN_RELFREQ</t>
+  </si>
+  <si>
+    <t>(float)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -171,6 +213,46 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Menlo Regular"/>
     </font>
   </fonts>
   <fills count="11">
@@ -244,10 +326,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -261,8 +345,34 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -573,7 +683,7 @@
         <v>21</v>
       </c>
       <c r="I1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -926,7 +1036,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B14">
         <v>187218</v>
@@ -1187,7 +1297,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1256,45 +1366,124 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:A8"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="1" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="D4" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
+      <c r="D8" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="21"/>
+    </row>
+    <row r="16" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="22">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="22">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="2:5" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>